<commit_message>
Stoneborn - Delights - 3106413957 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Stoneborn - Delights - 3106413957/Stoneborn - Delights - 3106413957.xlsx
+++ b/Data/Stoneborn - Delights - 3106413957/Stoneborn - Delights - 3106413957.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\Stoneborn - Delights - 3106413957\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB6CB50F-8BA2-4718-9598-7D58FE2D5744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753A0443-4B9B-4F7F-B328-2307796CB3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1655" uniqueCount="1168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1740" uniqueCount="1225">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -3707,6 +3720,182 @@
   </si>
   <si>
     <t>ThoughtDef+Inebriated.stages.quite_inebriated.label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HediffDef: SD_BullgrogHigh.label 'bullgrog high'</t>
+  </si>
+  <si>
+    <t>HediffDef: SD_BullgrogHigh.description 'Bullgrog is in the blood stream, it tastes kind of gross but gets you drunk fast, and makes you as hungry as a cow.'</t>
+  </si>
+  <si>
+    <t>HediffDef: SD_BullgrogHigh.labelNoun 'drunkenness'</t>
+  </si>
+  <si>
+    <t>HediffDef: SD_BullgrogHigh.stages.warm.label 'warm'</t>
+  </si>
+  <si>
+    <t>HediffDef: SD_BullgrogHigh.stages.tipsy.label 'tipsy'</t>
+  </si>
+  <si>
+    <t>HediffDef: SD_BullgrogHigh.stages.drunk.label 'drunk'</t>
+  </si>
+  <si>
+    <t>HediffDef: SD_BullgrogHigh.stages.hammered.label 'hammered'</t>
+  </si>
+  <si>
+    <t>HediffDef: SD_BullgrogHigh.stages.blackout.label 'blackout'</t>
+  </si>
+  <si>
+    <t>RecipeDef: Make_GlimmerCrystals.jobString 'Cutting stone blocks from chunk.'</t>
+  </si>
+  <si>
+    <t>ThoughtDef: BullgrogInebriated.stages.ale_warmth.label 'ale warmth'</t>
+  </si>
+  <si>
+    <t>ThoughtDef: BullgrogInebriated.stages.ale_warmth.description 'Yuck, this tastes gross.. but I'm feelin' good!'</t>
+  </si>
+  <si>
+    <t>ThoughtDef: BullgrogInebriated.stages.quite_inebriated.label 'quite inebriated'</t>
+  </si>
+  <si>
+    <t>ThoughtDef: BullgrogInebriated.stages.quite_inebriated.description 'I'm getting hungry, but I feel warmer!'</t>
+  </si>
+  <si>
+    <t>ThoughtDef: BullgrogInebriated.stages.drunk.label 'drunk'</t>
+  </si>
+  <si>
+    <t>ThoughtDef: BullgrogInebriated.stages.drunk.description 'God, now I'm really getting hungry..'</t>
+  </si>
+  <si>
+    <t>ThoughtDef: BullgrogInebriated.stages.hammered.label 'hammered'</t>
+  </si>
+  <si>
+    <t>ThoughtDef: BullgrogInebriated.stages.hammered.description 'I'm so hungry I could eat a whole browbull!'</t>
+  </si>
+  <si>
+    <t>SD_BullgrogHigh.label</t>
+  </si>
+  <si>
+    <t>SD_BullgrogHigh.description</t>
+  </si>
+  <si>
+    <t>SD_BullgrogHigh.labelNoun</t>
+  </si>
+  <si>
+    <t>SD_BullgrogHigh.stages.warm.label</t>
+  </si>
+  <si>
+    <t>SD_BullgrogHigh.stages.tipsy.label</t>
+  </si>
+  <si>
+    <t>SD_BullgrogHigh.stages.drunk.label</t>
+  </si>
+  <si>
+    <t>SD_BullgrogHigh.stages.hammered.label</t>
+  </si>
+  <si>
+    <t>SD_BullgrogHigh.stages.blackout.label</t>
+  </si>
+  <si>
+    <t>Make_GlimmerCrystals.jobString</t>
+  </si>
+  <si>
+    <t>BullgrogInebriated.stages.ale_warmth.label</t>
+  </si>
+  <si>
+    <t>BullgrogInebriated.stages.ale_warmth.description</t>
+  </si>
+  <si>
+    <t>BullgrogInebriated.stages.quite_inebriated.label</t>
+  </si>
+  <si>
+    <t>BullgrogInebriated.stages.quite_inebriated.description</t>
+  </si>
+  <si>
+    <t>BullgrogInebriated.stages.drunk.label</t>
+  </si>
+  <si>
+    <t>BullgrogInebriated.stages.drunk.description</t>
+  </si>
+  <si>
+    <t>BullgrogInebriated.stages.hammered.label</t>
+  </si>
+  <si>
+    <t>BullgrogInebriated.stages.hammered.description</t>
+  </si>
+  <si>
+    <t>bullgrog high'</t>
+  </si>
+  <si>
+    <t>Bullgrog is in the blood stream, it tastes kind of gross but gets you drunk fast, and makes you as hungry as a cow.'</t>
+  </si>
+  <si>
+    <t>drunkenness'</t>
+  </si>
+  <si>
+    <t>warm'</t>
+  </si>
+  <si>
+    <t>tipsy'</t>
+  </si>
+  <si>
+    <t>drunk'</t>
+  </si>
+  <si>
+    <t>hammered'</t>
+  </si>
+  <si>
+    <t>blackout'</t>
+  </si>
+  <si>
+    <t>Cutting stone blocks from chunk.'</t>
+  </si>
+  <si>
+    <t>ale warmth'</t>
+  </si>
+  <si>
+    <t>Yuck, this tastes gross.. but I'm feelin' good!'</t>
+  </si>
+  <si>
+    <t>quite inebriated'</t>
+  </si>
+  <si>
+    <t>I'm getting hungry, but I feel warmer!'</t>
+  </si>
+  <si>
+    <t>God, now I'm really getting hungry..'</t>
+  </si>
+  <si>
+    <t>I'm so hungry I could eat a whole browbull!'</t>
+  </si>
+  <si>
+    <t>불그록에 취함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>혈류의 불그록. 역겨운 맛이 나지만 빨리 취하고 소처럼 배가 고프게 만듭니다.</t>
+  </si>
+  <si>
+    <t>술 취함</t>
+  </si>
+  <si>
+    <t>글리머쿼츠 덩어리 자르는 중…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>역겨운 맛이야… 하지만 기분은 좋아!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배는 고프지만 몸은 더 따뜻하군!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>세상에, 이제 정말 배고파 죽겠네...</t>
+  </si>
+  <si>
+    <t>너무 배고파서 황소 한 마리를 통째로 먹을 수 있을 것 같아!</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4096,10 +4285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H330"/>
+  <dimension ref="A1:H347"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A266" workbookViewId="0">
-      <selection activeCell="C287" sqref="C287"/>
+    <sheetView tabSelected="1" topLeftCell="A317" workbookViewId="0">
+      <selection activeCell="D337" sqref="D337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -10721,6 +10910,363 @@
       <c r="G330" s="3"/>
       <c r="H330" s="3"/>
     </row>
+    <row r="331" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B331" t="s">
+        <v>269</v>
+      </c>
+      <c r="C331" t="s">
+        <v>1185</v>
+      </c>
+      <c r="D331" t="s">
+        <v>1202</v>
+      </c>
+      <c r="E331" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="F331" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G331" t="str">
+        <f>RIGHT(F331,LEN(F331)-FIND(" '",F331)-1)</f>
+        <v>bullgrog high'</v>
+      </c>
+    </row>
+    <row r="332" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B332" t="s">
+        <v>269</v>
+      </c>
+      <c r="C332" t="s">
+        <v>1186</v>
+      </c>
+      <c r="D332" t="s">
+        <v>1203</v>
+      </c>
+      <c r="E332" t="s">
+        <v>1218</v>
+      </c>
+      <c r="F332" t="s">
+        <v>1169</v>
+      </c>
+      <c r="G332" t="str">
+        <f t="shared" ref="G332:G347" si="0">RIGHT(F332,LEN(F332)-FIND(" '",F332)-1)</f>
+        <v>Bullgrog is in the blood stream, it tastes kind of gross but gets you drunk fast, and makes you as hungry as a cow.'</v>
+      </c>
+    </row>
+    <row r="333" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B333" t="s">
+        <v>269</v>
+      </c>
+      <c r="C333" t="s">
+        <v>1187</v>
+      </c>
+      <c r="D333" t="s">
+        <v>1204</v>
+      </c>
+      <c r="E333" t="s">
+        <v>1219</v>
+      </c>
+      <c r="F333" t="s">
+        <v>1170</v>
+      </c>
+      <c r="G333" t="str">
+        <f t="shared" si="0"/>
+        <v>drunkenness'</v>
+      </c>
+    </row>
+    <row r="334" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B334" t="s">
+        <v>269</v>
+      </c>
+      <c r="C334" t="s">
+        <v>1188</v>
+      </c>
+      <c r="D334" t="s">
+        <v>1205</v>
+      </c>
+      <c r="E334" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="F334" t="s">
+        <v>1171</v>
+      </c>
+      <c r="G334" t="str">
+        <f t="shared" si="0"/>
+        <v>warm'</v>
+      </c>
+    </row>
+    <row r="335" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B335" t="s">
+        <v>269</v>
+      </c>
+      <c r="C335" t="s">
+        <v>1189</v>
+      </c>
+      <c r="D335" t="s">
+        <v>1206</v>
+      </c>
+      <c r="E335" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="F335" t="s">
+        <v>1172</v>
+      </c>
+      <c r="G335" t="str">
+        <f t="shared" si="0"/>
+        <v>tipsy'</v>
+      </c>
+    </row>
+    <row r="336" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B336" t="s">
+        <v>269</v>
+      </c>
+      <c r="C336" t="s">
+        <v>1190</v>
+      </c>
+      <c r="D336" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E336" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="F336" t="s">
+        <v>1173</v>
+      </c>
+      <c r="G336" t="str">
+        <f t="shared" si="0"/>
+        <v>drunk'</v>
+      </c>
+    </row>
+    <row r="337" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B337" t="s">
+        <v>269</v>
+      </c>
+      <c r="C337" t="s">
+        <v>1191</v>
+      </c>
+      <c r="D337" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E337" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="F337" t="s">
+        <v>1174</v>
+      </c>
+      <c r="G337" t="str">
+        <f t="shared" si="0"/>
+        <v>hammered'</v>
+      </c>
+    </row>
+    <row r="338" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B338" t="s">
+        <v>269</v>
+      </c>
+      <c r="C338" t="s">
+        <v>1192</v>
+      </c>
+      <c r="D338" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E338" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="F338" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G338" t="str">
+        <f t="shared" si="0"/>
+        <v>blackout'</v>
+      </c>
+    </row>
+    <row r="339" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B339" t="s">
+        <v>817</v>
+      </c>
+      <c r="C339" t="s">
+        <v>1193</v>
+      </c>
+      <c r="D339" t="s">
+        <v>1210</v>
+      </c>
+      <c r="E339" s="1" t="s">
+        <v>1220</v>
+      </c>
+      <c r="F339" t="s">
+        <v>1176</v>
+      </c>
+      <c r="G339" t="str">
+        <f t="shared" si="0"/>
+        <v>Cutting stone blocks from chunk.'</v>
+      </c>
+    </row>
+    <row r="340" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B340" t="s">
+        <v>614</v>
+      </c>
+      <c r="C340" t="s">
+        <v>1194</v>
+      </c>
+      <c r="D340" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E340" s="1" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F340" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G340" t="str">
+        <f t="shared" si="0"/>
+        <v>ale warmth'</v>
+      </c>
+    </row>
+    <row r="341" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B341" t="s">
+        <v>614</v>
+      </c>
+      <c r="C341" t="s">
+        <v>1195</v>
+      </c>
+      <c r="D341" t="s">
+        <v>1212</v>
+      </c>
+      <c r="E341" s="1" t="s">
+        <v>1221</v>
+      </c>
+      <c r="F341" t="s">
+        <v>1178</v>
+      </c>
+      <c r="G341" t="str">
+        <f t="shared" si="0"/>
+        <v>Yuck, this tastes gross.. but I'm feelin' good!'</v>
+      </c>
+    </row>
+    <row r="342" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B342" t="s">
+        <v>614</v>
+      </c>
+      <c r="C342" t="s">
+        <v>1196</v>
+      </c>
+      <c r="D342" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E342" s="1" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F342" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G342" t="str">
+        <f t="shared" si="0"/>
+        <v>quite inebriated'</v>
+      </c>
+    </row>
+    <row r="343" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B343" t="s">
+        <v>614</v>
+      </c>
+      <c r="C343" t="s">
+        <v>1197</v>
+      </c>
+      <c r="D343" t="s">
+        <v>1214</v>
+      </c>
+      <c r="E343" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F343" t="s">
+        <v>1180</v>
+      </c>
+      <c r="G343" t="str">
+        <f t="shared" si="0"/>
+        <v>I'm getting hungry, but I feel warmer!'</v>
+      </c>
+    </row>
+    <row r="344" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B344" t="s">
+        <v>614</v>
+      </c>
+      <c r="C344" t="s">
+        <v>1198</v>
+      </c>
+      <c r="D344" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E344" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="F344" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G344" t="str">
+        <f t="shared" si="0"/>
+        <v>drunk'</v>
+      </c>
+    </row>
+    <row r="345" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B345" t="s">
+        <v>614</v>
+      </c>
+      <c r="C345" t="s">
+        <v>1199</v>
+      </c>
+      <c r="D345" t="s">
+        <v>1215</v>
+      </c>
+      <c r="E345" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F345" t="s">
+        <v>1182</v>
+      </c>
+      <c r="G345" t="str">
+        <f t="shared" si="0"/>
+        <v>God, now I'm really getting hungry..'</v>
+      </c>
+    </row>
+    <row r="346" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B346" t="s">
+        <v>614</v>
+      </c>
+      <c r="C346" t="s">
+        <v>1200</v>
+      </c>
+      <c r="D346" t="s">
+        <v>1208</v>
+      </c>
+      <c r="E346" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="F346" t="s">
+        <v>1183</v>
+      </c>
+      <c r="G346" t="str">
+        <f t="shared" si="0"/>
+        <v>hammered'</v>
+      </c>
+    </row>
+    <row r="347" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B347" t="s">
+        <v>614</v>
+      </c>
+      <c r="C347" t="s">
+        <v>1201</v>
+      </c>
+      <c r="D347" t="s">
+        <v>1216</v>
+      </c>
+      <c r="E347" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="F347" t="s">
+        <v>1184</v>
+      </c>
+      <c r="G347" t="str">
+        <f t="shared" si="0"/>
+        <v>I'm so hungry I could eat a whole browbull!'</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>